<commit_message>
added a lot of stuff
</commit_message>
<xml_diff>
--- a/Parameter_History.xlsx
+++ b/Parameter_History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziyangding\Desktop\TencentRecommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821FA75B-B357-4671-8C7E-A4F0CBFC93C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED3921E-7439-4581-A7B1-D6888D2F3029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12810" xr2:uid="{A8A5CF6B-1A7B-49BF-AA5C-DDB5794BC5B3}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>data_size</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>test AUC</t>
+  </si>
+  <si>
+    <t>num_decode_1</t>
+  </si>
+  <si>
+    <t>num_decode_2</t>
+  </si>
+  <si>
+    <t>num_decode_3</t>
+  </si>
+  <si>
+    <t>NAN</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Increasing alpha helps training a lot</t>
+  </si>
+  <si>
+    <t>0.65 (sometimes 0.72)</t>
   </si>
 </sst>
 </file>
@@ -107,8 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,110 +447,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF3F806-A024-4425-913F-1D4F325AA132}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="39.140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>20000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.01</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>512</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>256</v>
       </c>
-      <c r="F2">
-        <v>124</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="1">
+        <v>128</v>
+      </c>
+      <c r="G2" s="1">
         <v>64</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>32</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>16</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
+        <v>128</v>
+      </c>
+      <c r="L2" s="1">
+        <v>256</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="O2" s="1">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="P2" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="N2">
+      <c r="Q2" s="1">
         <v>0.70003800000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2048</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>128</v>
+      </c>
+      <c r="F3" s="1">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1">
+        <v>64</v>
+      </c>
+      <c r="M3" s="1">
+        <v>128</v>
+      </c>
+      <c r="N3" s="1">
+        <v>8</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>